<commit_message>
Added new invoice file for testing
</commit_message>
<xml_diff>
--- a/Labfiles/01-prebuild-models/results/testing.xlsx
+++ b/Labfiles/01-prebuild-models/results/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DocToExcel2\DocToExcel\Labfiles\01-prebuild-models\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E77A129-0EBF-47E0-9F38-2073CA6E11DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3FF195-9810-4CB5-B7CD-AA797A6F6D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,11 +528,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E79E6A7-0F89-4EFE-8AC2-32BDB009BAD3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56240AFB-6A15-4EC4-8161-C6283DFB606C}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Added combined pdf for testing purposes
</commit_message>
<xml_diff>
--- a/Labfiles/01-prebuild-models/results/testing.xlsx
+++ b/Labfiles/01-prebuild-models/results/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DocToExcel2\DocToExcel\Labfiles\01-prebuild-models\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3FF195-9810-4CB5-B7CD-AA797A6F6D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EC28D5-5FC7-413F-98C3-1FA1C9691C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56240AFB-6A15-4EC4-8161-C6283DFB606C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F3B92C-B786-4FBF-A765-5A4547966888}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Changes to invoice files
</commit_message>
<xml_diff>
--- a/Labfiles/01-prebuild-models/results/testing.xlsx
+++ b/Labfiles/01-prebuild-models/results/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DocToExcel2\DocToExcel\Labfiles\01-prebuild-models\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EC28D5-5FC7-413F-98C3-1FA1C9691C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A479E-6F6B-4EF2-A032-9CF8F251B4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>ALL LEDGERS</t>
   </si>
@@ -84,13 +84,7 @@
     <t>I</t>
   </si>
   <si>
-    <t>IN23/12651</t>
-  </si>
-  <si>
-    <t>Cleaning Service 4 Hrs 2 Persons</t>
-  </si>
-  <si>
-    <t>Infinity Wave Sdn Bhd</t>
+    <t>Monthly meeting</t>
   </si>
 </sst>
 </file>
@@ -528,7 +522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F3B92C-B786-4FBF-A765-5A4547966888}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93147FC2-9EB3-450E-9400-1834E06354B9}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -618,22 +612,19 @@
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="11">
-        <v>45031</v>
+        <v>44737</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1">
+        <v>12345</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K10" s="1">
-        <v>180</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1"/>

</xml_diff>

<commit_message>
Changes to invoice pdf
</commit_message>
<xml_diff>
--- a/Labfiles/01-prebuild-models/results/testing.xlsx
+++ b/Labfiles/01-prebuild-models/results/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DocToExcel2\DocToExcel\Labfiles\01-prebuild-models\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A479E-6F6B-4EF2-A032-9CF8F251B4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588C3DA5-BF93-44FE-9886-224872139E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>ALL LEDGERS</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>MYR</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>Monthly meeting</t>
   </si>
 </sst>
 </file>
@@ -154,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -174,7 +168,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93147FC2-9EB3-450E-9400-1834E06354B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8969F2-6946-4498-8898-DBA08196D9E6}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -610,23 +603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="11">
-        <v>44737</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1">
-        <v>12345</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="1">
-        <v>2000</v>
-      </c>
-    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1"/>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1"/>
     <row r="12" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1"/>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1"/>

</xml_diff>

<commit_message>
Uploading actual test files
</commit_message>
<xml_diff>
--- a/Labfiles/01-prebuild-models/results/testing.xlsx
+++ b/Labfiles/01-prebuild-models/results/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DocToExcel2\DocToExcel\Labfiles\01-prebuild-models\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B287C0D-18B8-4DA8-82E4-B79CBEF87087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A586F3-3BA1-4410-B34C-C15ED8E7A31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>